<commit_message>
Added  qa fixes - 10/31/2017
</commit_message>
<xml_diff>
--- a/PLMVCSolution/PL.MVC.IOBalanceV2/Content/excel/templates/BatchInventoryTemplate.xlsx
+++ b/PLMVCSolution/PL.MVC.IOBalanceV2/Content/excel/templates/BatchInventoryTemplate.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lloyd Martinez\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="ColTemplate - 01" sheetId="2" r:id="rId2"/>
+    <sheet name="ColTemplate - 01" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="PLUS_MINUSRANGE">'ColTemplate - 01'!$A$1:$A$2</definedName>
     <definedName name="Y_N_RANGE">'ColTemplate - 01'!$B$1:$B$2</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>PRODUCT_CODE</t>
   </si>
@@ -65,34 +70,10 @@
     <t>IS_NEW</t>
   </si>
   <si>
-    <t>PROD100</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>HASUS SHOES</t>
-  </si>
-  <si>
-    <t>TS1</t>
-  </si>
-  <si>
-    <t>PCS</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>9</t>
   </si>
   <si>
     <t>-</t>
@@ -104,8 +85,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,10 +122,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,21 +433,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -476,7 +465,7 @@
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,81 +506,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>20</v>
-      </c>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>PLUS_MINUSRANGE</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Y_N_RANGE</formula1>
     </dataValidation>
   </dataValidations>
@@ -601,32 +530,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>